<commit_message>
op bitflip + depol 6qbit
</commit_message>
<xml_diff>
--- a/noise_Bitflip_1_to_6_qubits_pes.xlsx
+++ b/noise_Bitflip_1_to_6_qubits_pes.xlsx
@@ -508,38 +508,38 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>95.13</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>95.3</v>
+        <v>99.79000000000001</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>95.86</v>
+        <v>99.47</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>94.98999999999999</v>
+        <v>99.09</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>95</v>
+        <v>98.8</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>94.97</v>
+        <v>98.94</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>95.26000000000001</v>
+        <v>98.48</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>95.45</v>
+        <v>98.19</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>95.03</v>
+        <v>98.12</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>95.08</v>
+        <v>97.59</v>
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>95.38</t>
+          <t>97.7</t>
         </is>
       </c>
     </row>
@@ -548,38 +548,38 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>50.92</v>
+        <v>49.88</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>49.45</v>
+        <v>49.86</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>50.31</v>
+        <v>49.89</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>49.56</v>
+        <v>50.39</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>50.9</v>
+        <v>48.89</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>50.03999999999999</v>
+        <v>50.1</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>49.53</v>
+        <v>50.2</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>48.84</v>
+        <v>49.93</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>50.63999999999999</v>
+        <v>50.13999999999999</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>50.33</v>
+        <v>49.67</v>
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>50.160000000000004</t>
+          <t>50.39</t>
         </is>
       </c>
     </row>
@@ -669,38 +669,38 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>2.102386208346473</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>2.098635886673662</v>
+        <v>2.004208838560978</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2.086375964948884</v>
+        <v>2.010656479340505</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>2.105484787872407</v>
+        <v>2.018367140982945</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>2.105263157894737</v>
+        <v>2.024291497975709</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>2.105928187848794</v>
+        <v>2.021427127552052</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>2.099517111064455</v>
+        <v>2.030869212022746</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>2.095337873232059</v>
+        <v>2.036867298095529</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>2.104598547827002</v>
+        <v>2.038320423970648</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2.103491796381994</v>
+        <v>2.049390306383851</v>
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>2.0968756552736423</t>
+          <t>2.0470829068577276</t>
         </is>
       </c>
     </row>
@@ -709,38 +709,38 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>3.927729772191673</v>
+        <v>4.00962309542903</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>4.044489383215369</v>
+        <v>4.011231448054553</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>3.975352812562115</v>
+        <v>4.008819402685909</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>4.035512510088782</v>
+        <v>3.969041476483429</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>3.929273084479371</v>
+        <v>4.090816117815504</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>3.996802557953637</v>
+        <v>3.992015968063872</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>4.037956793862306</v>
+        <v>3.98406374501992</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>4.095004095004095</v>
+        <v>4.005607850991388</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>3.949447077409163</v>
+        <v>3.988831272437176</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>3.973773097556129</v>
+        <v>4.02657539762432</v>
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>3.9872408293460926</t>
+          <t>3.9690414764834294</t>
         </is>
       </c>
     </row>
@@ -830,38 +830,38 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>57.84</v>
+        <v>94.27</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>58.84</v>
+        <v>91.81</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>56.48</v>
+        <v>89.25</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>59.07</v>
+        <v>86.89</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>57.67</v>
+        <v>86.52</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>56.89999999999999</v>
+        <v>82.04000000000001</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>57.9</v>
+        <v>81.82000000000001</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>57.98</v>
+        <v>79.21000000000001</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>58.34</v>
+        <v>77.31</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>56.27</v>
+        <v>75.98</v>
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>59.12</t>
+          <t>73.19</t>
         </is>
       </c>
     </row>
@@ -870,38 +870,38 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>78.56</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>77.72</v>
+        <v>98.59999999999999</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>78.28</v>
+        <v>97.8</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>81.56</v>
+        <v>95.81999999999999</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>77.40000000000001</v>
+        <v>95.34</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>80.25</v>
+        <v>93.62</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>80.60000000000001</v>
+        <v>91.88</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>76.06</v>
+        <v>91.28</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>79.66</v>
+        <v>90.54000000000001</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>78.18000000000001</v>
+        <v>90.36</v>
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>78.68</t>
+          <t>87.72999999999999</t>
         </is>
       </c>
     </row>
@@ -910,38 +910,38 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>69.31</v>
+        <v>84.50999999999999</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>71.76000000000001</v>
+        <v>83.77</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>70.3</v>
+        <v>82.83</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>69.8</v>
+        <v>81.55</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>69.87</v>
+        <v>80.98999999999999</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>70.8</v>
+        <v>80.17</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>70.08</v>
+        <v>79.25</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>69.58</v>
+        <v>79.03999999999999</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>70.19999999999999</v>
+        <v>77.91</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>71.26000000000001</v>
+        <v>77.97</v>
       </c>
       <c r="L4" s="2" t="inlineStr">
         <is>
-          <t>69.98</t>
+          <t>76.94</t>
         </is>
       </c>
     </row>
@@ -950,38 +950,38 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>50.6</v>
+        <v>49.44</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>49.13</v>
+        <v>49.87</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>49.59</v>
+        <v>50.19</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>50.02</v>
+        <v>49.77</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>49.85</v>
+        <v>50.11</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>50.02</v>
+        <v>50.42</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>50.13999999999999</v>
+        <v>49.17</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>49.2</v>
+        <v>50.48</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>50.23</v>
+        <v>49.99</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>48.94</v>
+        <v>50.32</v>
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>50.0</t>
+          <t>50.980000000000004</t>
         </is>
       </c>
     </row>
@@ -1071,38 +1071,38 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>5.186721991701245</v>
+        <v>3.182348573247056</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>5.098572399728076</v>
+        <v>3.267617906546127</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5.311614730878187</v>
+        <v>3.361344537815126</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>5.078720162519045</v>
+        <v>3.452641270571988</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>5.202011444425177</v>
+        <v>3.467406380027739</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>5.272407732864675</v>
+        <v>3.656752803510482</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>5.181347150259067</v>
+        <v>3.666585186995845</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>5.174197999310107</v>
+        <v>3.787400580734755</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>5.142269454919438</v>
+        <v>3.880481179666279</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>5.331437711036076</v>
+        <v>3.948407475651488</v>
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>5.074424898511502</t>
+          <t>4.098920617570706</t>
         </is>
       </c>
     </row>
@@ -1111,38 +1111,38 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>2.545824847250509</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>2.573340195573855</v>
+        <v>2.028397565922921</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>2.554931016862545</v>
+        <v>2.044989775051125</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>2.452182442373712</v>
+        <v>2.087246921310791</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>2.583979328165375</v>
+        <v>2.09775540172016</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>2.49221183800623</v>
+        <v>2.136295663319804</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>2.481389578163772</v>
+        <v>2.1767522855899</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>2.629503023928478</v>
+        <v>2.191060473269062</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>2.510670348983179</v>
+        <v>2.208968411751712</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>2.55819902788437</v>
+        <v>2.213368747233289</v>
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>2.541942043721403</t>
+          <t>2.2797218739313805</t>
         </is>
       </c>
     </row>
@@ -1151,38 +1151,38 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>2.885586495455201</v>
+        <v>2.366583836232398</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>2.787068004459309</v>
+        <v>2.387489554733198</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2.844950213371266</v>
+        <v>2.414584087890861</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2.865329512893983</v>
+        <v>2.452483139178418</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>2.862458852154</v>
+        <v>2.469440671687863</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>2.824858757062147</v>
+        <v>2.494698765124112</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>2.853881278538813</v>
+        <v>2.523659305993691</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>2.874389192296637</v>
+        <v>2.530364372469636</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>2.849002849002849</v>
+        <v>2.567064561673726</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>2.80662363177098</v>
+        <v>2.565089136847505</v>
       </c>
       <c r="L4" s="2" t="inlineStr">
         <is>
-          <t>2.857959416976279</t>
+          <t>2.599428125812321</t>
         </is>
       </c>
     </row>
@@ -1191,38 +1191,38 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>3.952569169960474</v>
+        <v>4.045307443365696</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>4.070832485243232</v>
+        <v>4.010427110487267</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>4.033071183706393</v>
+        <v>3.984857541342897</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>3.998400639744102</v>
+        <v>4.018485031143259</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>4.012036108324975</v>
+        <v>3.991219317501497</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>3.998400639744102</v>
+        <v>3.966679888932963</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>3.988831272437176</v>
+        <v>4.067520846044336</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>4.065040650406504</v>
+        <v>3.961965134706815</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>3.981684252438781</v>
+        <v>4.000800160032006</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>4.086636697997548</v>
+        <v>3.97456279809221</v>
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.9231071008238523</t>
         </is>
       </c>
     </row>
@@ -1312,38 +1312,38 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>13.47</v>
+        <v>90.45</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>14.21</v>
+        <v>80.75</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>12.49</v>
+        <v>70.82000000000001</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>12.65</v>
+        <v>61.63</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>12.99</v>
+        <v>56.7</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>11.95</v>
+        <v>48.29</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>12.38</v>
+        <v>44.41</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>13.38</v>
+        <v>40.28</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>12.58</v>
+        <v>36.05</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>12.43</v>
+        <v>32.02999999999999</v>
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>12.78</t>
+          <t>26.8</t>
         </is>
       </c>
     </row>
@@ -1352,38 +1352,38 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>19.43</v>
+        <v>94.77</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>16.12</v>
+        <v>82.86</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>17.8</v>
+        <v>73.63</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>16.43</v>
+        <v>64.8</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>15.39</v>
+        <v>54.66</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>16.61</v>
+        <v>48.14</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>19.04</v>
+        <v>44.74</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>17.2</v>
+        <v>43.11</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>15.75</v>
+        <v>36.59</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>16.84</v>
+        <v>32.27</v>
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>16.220000000000002</t>
+          <t>31.56</t>
         </is>
       </c>
     </row>
@@ -1392,38 +1392,38 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>32.78</v>
+        <v>94.98999999999999</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>31.97</v>
+        <v>88.73</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>32.95</v>
+        <v>83.54000000000001</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>33.41</v>
+        <v>78.75999999999999</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>31.88</v>
+        <v>72.55</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>32.42</v>
+        <v>66.64999999999999</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>34.98</v>
+        <v>63.49</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>34.36</v>
+        <v>57.75</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>33.7</v>
+        <v>56.21000000000001</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>32.54</v>
+        <v>52.40000000000001</v>
       </c>
       <c r="L4" s="2" t="inlineStr">
         <is>
-          <t>33.57</t>
+          <t>50.71</t>
         </is>
       </c>
     </row>
@@ -1432,38 +1432,38 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>37.82</v>
+        <v>100</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>36.98</v>
+        <v>93.52</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>38.99</v>
+        <v>87.94</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>36.68</v>
+        <v>82.19</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>38.2</v>
+        <v>76.95999999999999</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>40.04</v>
+        <v>72.7</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>36.95</v>
+        <v>67.89</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>37.75</v>
+        <v>65.8</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>38.63</v>
+        <v>62.28</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>38.36</v>
+        <v>57.19</v>
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>37.03</t>
+          <t>55.900000000000006</t>
         </is>
       </c>
     </row>
@@ -1472,38 +1472,38 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>41.62</v>
+        <v>95.41</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>41.89</v>
+        <v>89.8</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>43.89</v>
+        <v>84.55</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>41.54</v>
+        <v>80.51000000000001</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>42.44</v>
+        <v>76.12</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>41.75</v>
+        <v>71.17</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>41.72</v>
+        <v>67.52</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>42.41</v>
+        <v>66.32000000000001</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>40.84</v>
+        <v>62.28</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>41.76000000000001</v>
+        <v>60.07</v>
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>40.8</t>
+          <t>57.64</t>
         </is>
       </c>
     </row>
@@ -1512,38 +1512,38 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44.93</v>
+        <v>84.06999999999999</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45.22</v>
+        <v>80.38</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>45.01</v>
+        <v>75.25</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>45.72</v>
+        <v>73.08</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>44.93</v>
+        <v>69.76000000000001</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>44.98</v>
+        <v>65.64999999999999</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>44.9</v>
+        <v>64.33</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>46.33</v>
+        <v>61.74</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>44.82</v>
+        <v>59.73</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>45.13</v>
+        <v>58.81999999999999</v>
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>44.800000000000004</t>
+          <t>55.33</t>
         </is>
       </c>
     </row>
@@ -1552,38 +1552,38 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>47.85</v>
+        <v>69</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>47.76000000000001</v>
+        <v>66.13</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>48.96</v>
+        <v>64.78</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>47.24</v>
+        <v>61.56</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>49</v>
+        <v>61.71</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>46.68</v>
+        <v>58.7</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>47.58</v>
+        <v>58.54000000000001</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>48</v>
+        <v>55.2</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>47.41</v>
+        <v>54.91</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>47.55</v>
+        <v>53.90000000000001</v>
       </c>
       <c r="L8" s="2" t="inlineStr">
         <is>
-          <t>48.52</t>
+          <t>54.43</t>
         </is>
       </c>
     </row>
@@ -1592,38 +1592,38 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="n">
+        <v>50.95</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>50.2</v>
+      </c>
+      <c r="D9" s="2" t="n">
         <v>50.27</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>49.67</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>50.22</v>
-      </c>
       <c r="E9" s="2" t="n">
-        <v>49.56</v>
+        <v>49.75</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>50.72</v>
+        <v>49.96</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>50.24</v>
+        <v>50.07</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>49.49</v>
+        <v>49.21</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>50.69</v>
+        <v>50.17</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>49.49</v>
+        <v>49.36</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>50.67</v>
+        <v>50.54</v>
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>49.82</t>
+          <t>50.56</t>
         </is>
       </c>
     </row>
@@ -1713,38 +1713,38 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>22.271714922049</v>
+        <v>3.316749585406302</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>21.1118930330753</v>
+        <v>3.715170278637771</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>24.01921537229784</v>
+        <v>4.236091499576391</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>23.71541501976284</v>
+        <v>4.867759208177835</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>23.09468822170901</v>
+        <v>5.291005291005291</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>25.10460251046025</v>
+        <v>6.212466349140609</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>24.23263327948304</v>
+        <v>6.755235307363206</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>22.42152466367713</v>
+        <v>7.447864945382323</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>23.84737678855326</v>
+        <v>8.321775312066574</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>24.13515687851971</v>
+        <v>9.366219169528566</v>
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>23.474178403755868</t>
+          <t>11.194029850746269</t>
         </is>
       </c>
     </row>
@@ -1753,38 +1753,38 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>15.44004117344313</v>
+        <v>3.165558721114277</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>18.61042183622829</v>
+        <v>3.620564808110065</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>16.85393258426966</v>
+        <v>4.074426184978948</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>18.25928180158247</v>
+        <v>4.62962962962963</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>19.49317738791423</v>
+        <v>5.488474204171241</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>18.06140878988561</v>
+        <v>6.231823847112588</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>15.7563025210084</v>
+        <v>6.705409029950827</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>17.44186046511628</v>
+        <v>6.958942240779401</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>19.04761904761905</v>
+        <v>8.198961464881116</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>17.81472684085511</v>
+        <v>9.2965602726991</v>
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>18.495684340320594</t>
+          <t>9.505703422053232</t>
         </is>
       </c>
     </row>
@@ -1793,38 +1793,38 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>6.101281269066504</v>
+        <v>2.105484787872407</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>6.255864873318736</v>
+        <v>2.254029076975093</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>6.06980273141123</v>
+        <v>2.39406272444338</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>5.986231667165519</v>
+        <v>2.539360081259523</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>6.273525721455458</v>
+        <v>2.756719503790489</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>6.169031462060457</v>
+        <v>3.000750187546887</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>5.717552887364208</v>
+        <v>3.150102378327296</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>5.820721769499418</v>
+        <v>3.463203463203463</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>5.934718100890208</v>
+        <v>3.558085749866572</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>6.146281499692686</v>
+        <v>3.816793893129771</v>
       </c>
       <c r="L4" s="2" t="inlineStr">
         <is>
-          <t>5.957700327673518</t>
+          <t>3.9439952672056795</t>
         </is>
       </c>
     </row>
@@ -1833,38 +1833,38 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>5.288207297726071</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>5.408328826392645</v>
+        <v>2.13857998289136</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>5.12952038984355</v>
+        <v>2.274277916761428</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>5.452562704471101</v>
+        <v>2.433386056697896</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>5.235602094240837</v>
+        <v>2.598752598752599</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>4.995004995004995</v>
+        <v>2.751031636863824</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>5.412719891745602</v>
+        <v>2.945941964943291</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>5.298013245033113</v>
+        <v>3.03951367781155</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>5.177323323841574</v>
+        <v>3.211303789338471</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>5.213764337851929</v>
+        <v>3.497114880223815</v>
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>5.401026194977046</t>
+          <t>3.5778175313059033</t>
         </is>
       </c>
     </row>
@@ -1873,38 +1873,38 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>4.805382027871215</v>
+        <v>2.096216329525207</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>4.774409166865601</v>
+        <v>2.2271714922049</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>4.55684666210982</v>
+        <v>2.365464222353637</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>4.814636494944632</v>
+        <v>2.484163457955534</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>4.71253534401508</v>
+        <v>2.627430373095113</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>4.790419161676646</v>
+        <v>2.810172825628776</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>4.793863854266539</v>
+        <v>2.962085308056872</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>4.715868898844612</v>
+        <v>3.015681544028951</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>4.897159647404505</v>
+        <v>3.211303789338471</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>4.789272030651341</v>
+        <v>3.32944897619444</v>
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>4.901960784313726</t>
+          <t>3.4698126301179735</t>
         </is>
       </c>
     </row>
@@ -1913,38 +1913,38 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>4.451368795904741</v>
+        <v>2.378969906030689</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>4.42282176028306</v>
+        <v>2.488181139586962</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>4.443457009553432</v>
+        <v>2.6578073089701</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>4.374453193350831</v>
+        <v>2.736726874657909</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>4.451368795904741</v>
+        <v>2.86697247706422</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>4.44642063139173</v>
+        <v>3.046458492003046</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>4.4543429844098</v>
+        <v>3.10896937665164</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.316857327865314</v>
+        <v>3.239390994493035</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>4.462293618920125</v>
+        <v>3.348401138456387</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>4.431641923332594</v>
+        <v>3.400204012240735</v>
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>4.464285714285714</t>
+          <t>3.614675582866438</t>
         </is>
       </c>
     </row>
@@ -1953,38 +1953,38 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>4.179728317659352</v>
+        <v>2.898550724637681</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>4.187604690117253</v>
+        <v>3.024345985180705</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>4.084967320261438</v>
+        <v>3.087372645878358</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>4.233700254022016</v>
+        <v>3.248862897985705</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>4.081632653061225</v>
+        <v>3.240965807810728</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>4.284490145672665</v>
+        <v>3.407155025553663</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>4.203446826397646</v>
+        <v>3.41646737273659</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>4.166666666666667</v>
+        <v>3.623188405797102</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>4.218519299725796</v>
+        <v>3.64232380258605</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>4.206098843322818</v>
+        <v>3.710575139146568</v>
       </c>
       <c r="L8" s="2" t="inlineStr">
         <is>
-          <t>4.122011541632316</t>
+          <t>3.6744442403086532</t>
         </is>
       </c>
     </row>
@@ -1993,38 +1993,38 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="n">
+        <v>3.925417075564279</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>3.98406374501992</v>
+      </c>
+      <c r="D9" s="2" t="n">
         <v>3.978516013526955</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>4.02657539762432</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>3.982477100756671</v>
-      </c>
       <c r="E9" s="2" t="n">
-        <v>4.035512510088782</v>
+        <v>4.020100502512562</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>3.943217665615142</v>
+        <v>4.00320256204964</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>3.980891719745223</v>
+        <v>3.994407829039345</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>4.04122044857547</v>
+        <v>4.06421459053038</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>3.945551390806865</v>
+        <v>3.986446083316723</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>4.04122044857547</v>
+        <v>4.051863857374392</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>3.947108742845865</v>
+        <v>3.957261574990107</v>
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>4.014452027298274</t>
+          <t>3.9556962025316458</t>
         </is>
       </c>
     </row>
@@ -2039,7 +2039,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2083,29 +2083,69 @@
           <t>0.0025 noise level</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>0.003 noise level</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>0.0035 noise level</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>0.004 noise level</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>0.0045000000000000005 noise level</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>0.005 noise level</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>3.04</v>
+        <v>89.78</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>3.14</v>
+        <v>41.88</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3.28</v>
+        <v>18.66</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>2.96</v>
+        <v>11.21</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>3.08</v>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>3.1</t>
+        <v>5.680000000000001</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>4.590000000000001</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>3.54</t>
         </is>
       </c>
     </row>
@@ -2114,23 +2154,38 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>6.81</v>
+        <v>90.86</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>6.05</v>
+        <v>49.3</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>6.16</v>
+        <v>26.57</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>6.29</v>
+        <v>19.06</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>6.619999999999999</v>
-      </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>6.15</t>
+        <v>12.68</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>8.77</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>7.61</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>7.470000000000001</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>6.77</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>6.819999999999999</v>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>6.59</t>
         </is>
       </c>
     </row>
@@ -2139,23 +2194,38 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>9.17</v>
+        <v>99.97</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>8.859999999999999</v>
+        <v>50.81</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>9.49</v>
+        <v>30.7</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>9.81</v>
+        <v>19.23</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>9.119999999999999</v>
-      </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>9.67</t>
+        <v>14.7</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>12.33</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>10.56</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>10.17</v>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
+        <is>
+          <t>9.229999999999999</t>
         </is>
       </c>
     </row>
@@ -2164,23 +2234,38 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>12.49</v>
+        <v>94.29000000000001</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>12.44</v>
+        <v>51.13999999999999</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>12.37</v>
+        <v>29.87</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>12.09</v>
+        <v>20.61</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>13.31</v>
-      </c>
-      <c r="G5" s="2" t="inlineStr">
-        <is>
-          <t>13.04</t>
+        <v>16.08</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>13.91</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>13.12</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>12.79</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>13.4</v>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>12.18</t>
         </is>
       </c>
     </row>
@@ -2189,23 +2274,38 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>16.44</v>
+        <v>88.05</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>15.56</v>
+        <v>62.86000000000001</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>15.32</v>
+        <v>46.7</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>15.44</v>
+        <v>37.4</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>15.83</v>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>15.32</t>
+        <v>29.63</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>25.19</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>22.18</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>19.15</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>17.87</v>
+      </c>
+      <c r="L6" s="2" t="inlineStr">
+        <is>
+          <t>16.21</t>
         </is>
       </c>
     </row>
@@ -2214,23 +2314,38 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>18.51</v>
+        <v>94.84999999999999</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>19</v>
+        <v>68.28999999999999</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>19.55</v>
+        <v>50.79</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>18.24</v>
+        <v>39.68</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>18.85</v>
-      </c>
-      <c r="G7" s="2" t="inlineStr">
-        <is>
-          <t>19.580000000000002</t>
+        <v>31.62</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>29.17</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>23.18</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>23.16</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>21.63</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>20.61</v>
+      </c>
+      <c r="L7" s="2" t="inlineStr">
+        <is>
+          <t>19.759999999999998</t>
         </is>
       </c>
     </row>
@@ -2239,23 +2354,38 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>22.07</v>
+        <v>98.84</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>21.9</v>
+        <v>70.59</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>21.38</v>
+        <v>54.40000000000001</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>21.11</v>
+        <v>44.65</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>22.57</v>
-      </c>
-      <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>22.48</t>
+        <v>35.24</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>29.74</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>27.79</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>25.55</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>24.43</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>23.48</v>
+      </c>
+      <c r="L8" s="2" t="inlineStr">
+        <is>
+          <t>22.96</t>
         </is>
       </c>
     </row>
@@ -2264,23 +2394,38 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>24.69</v>
+        <v>100</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>25.32</v>
+        <v>73.05</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>25.23</v>
+        <v>56.11000000000001</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>25.51</v>
+        <v>45.38</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>25.06</v>
-      </c>
-      <c r="G9" s="2" t="inlineStr">
-        <is>
-          <t>25.64</t>
+        <v>37.78</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>33.12</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>30.58</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>29.12</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>27.74</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>26.76</v>
+      </c>
+      <c r="L9" s="2" t="inlineStr">
+        <is>
+          <t>26.02</t>
         </is>
       </c>
     </row>
@@ -2289,23 +2434,38 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>28.09</v>
+        <v>98.87</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>28.45</v>
+        <v>72.70999999999999</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>29.35</v>
+        <v>57.15</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>28.64</v>
+        <v>46.6</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>28.49</v>
-      </c>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>28.84</t>
+        <v>39.72</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>36.38</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>32.79</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>32.18</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>30.41</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>30.34</v>
+      </c>
+      <c r="L10" s="2" t="inlineStr">
+        <is>
+          <t>28.54</t>
         </is>
       </c>
     </row>
@@ -2314,23 +2474,38 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>31.4</v>
+        <v>95.42</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>30.89</v>
+        <v>71.89</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>31.5</v>
+        <v>58.47</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>31.28</v>
+        <v>48.63</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>30.93</v>
-      </c>
-      <c r="G11" s="2" t="inlineStr">
-        <is>
-          <t>31.19</t>
+        <v>42.5</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>38.71</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>34.84999999999999</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>34.22</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>33.02</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>32.29</v>
+      </c>
+      <c r="L11" s="2" t="inlineStr">
+        <is>
+          <t>32.49</t>
         </is>
       </c>
     </row>
@@ -2339,23 +2514,38 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>34.08</v>
+        <v>91.02</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>34.54</v>
+        <v>70.19</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>34.34</v>
+        <v>56.69</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>34.55</v>
+        <v>48.98</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>34.05</v>
-      </c>
-      <c r="G12" s="2" t="inlineStr">
-        <is>
-          <t>33.660000000000004</t>
+        <v>43.51</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>40.69</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>37.72</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>37.28</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>36.14</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>34.79</v>
+      </c>
+      <c r="L12" s="2" t="inlineStr">
+        <is>
+          <t>35.69</t>
         </is>
       </c>
     </row>
@@ -2364,23 +2554,38 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>37.18</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>37.62</v>
+        <v>67.45</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>38.04</v>
+        <v>56.99</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>37.88</v>
+        <v>49.42</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>37.34</v>
-      </c>
-      <c r="G13" s="2" t="inlineStr">
-        <is>
-          <t>38.42</t>
+        <v>46.06</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>41.74</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>40.77</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>39.42</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>38.23</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>37.75</v>
+      </c>
+      <c r="L13" s="2" t="inlineStr">
+        <is>
+          <t>38.519999999999996</t>
         </is>
       </c>
     </row>
@@ -2389,23 +2594,38 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>39.38</v>
+        <v>77.10000000000001</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>40.69</v>
+        <v>63.29</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>40.40000000000001</v>
+        <v>55.81</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>40.57</v>
+        <v>51.27</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>40.75</v>
-      </c>
-      <c r="G14" s="2" t="inlineStr">
-        <is>
-          <t>40.9</t>
+        <v>46.75</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>44.69</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>43.19</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>42.13</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>40.15000000000001</v>
+      </c>
+      <c r="L14" s="2" t="inlineStr">
+        <is>
+          <t>40.660000000000004</t>
         </is>
       </c>
     </row>
@@ -2414,23 +2634,38 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>43.54</v>
+        <v>69</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>43.87</v>
+        <v>58.84</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>43.41</v>
+        <v>53.71</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>43.72</v>
+        <v>49.73</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>43.62</v>
-      </c>
-      <c r="G15" s="2" t="inlineStr">
-        <is>
-          <t>43.62</t>
+        <v>47.09</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>46.34</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>44.8</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>44.82</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>44.49</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>43.68</v>
+      </c>
+      <c r="L15" s="2" t="inlineStr">
+        <is>
+          <t>44.61</t>
         </is>
       </c>
     </row>
@@ -2439,23 +2674,38 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>47.22</v>
+        <v>59.54000000000001</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>47.19</v>
+        <v>54.82</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>46.65000000000001</v>
+        <v>51.33</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>45.81</v>
+        <v>50.17</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>46.93</v>
-      </c>
-      <c r="G16" s="2" t="inlineStr">
-        <is>
-          <t>46.89</t>
+        <v>48.31</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>48.25</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>47.62</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>47.69</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>47.58</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>46.7</v>
+      </c>
+      <c r="L16" s="2" t="inlineStr">
+        <is>
+          <t>47.21</t>
         </is>
       </c>
     </row>
@@ -2464,23 +2714,38 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>50.54</v>
+        <v>50.21</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>50.43</v>
+        <v>49.75</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>50.67</v>
+        <v>49.56</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>49.62</v>
+        <v>49.42</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>49.97</v>
-      </c>
-      <c r="G17" s="2" t="inlineStr">
-        <is>
-          <t>49.730000000000004</t>
+        <v>49.85</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>49.83000000000001</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>50.51</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>50.92</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>50.74999999999999</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>49.63</v>
+      </c>
+      <c r="L17" s="2" t="inlineStr">
+        <is>
+          <t>49.64</t>
         </is>
       </c>
     </row>
@@ -2495,7 +2760,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2539,29 +2804,69 @@
           <t>0.0025 noise level oracle calls</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>0.003 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>0.0035 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>0.004 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>0.0045000000000000005 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>0.005 noise level oracle calls</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>131.578947368421</v>
+        <v>4.455335263978615</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>127.3885350318471</v>
+        <v>9.551098376313275</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>121.9512195121951</v>
+        <v>21.43622722400858</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>135.1351351351351</v>
+        <v>35.68242640499554</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>129.8701298701299</v>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>129.03225806451613</t>
+        <v>70.4225352112676</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>87.14596949891067</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>94.56264775413712</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>109.2896174863388</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>122.3241590214067</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>126.984126984127</v>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>112.99435028248588</t>
         </is>
       </c>
     </row>
@@ -2570,23 +2875,38 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44.05286343612335</v>
+        <v>3.301782962799912</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>49.58677685950413</v>
+        <v>6.085192697768763</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>48.7012987012987</v>
+        <v>11.29092961987204</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>47.69475357710652</v>
+        <v>15.73976915005246</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45.31722054380664</v>
-      </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>48.78048780487805</t>
+        <v>23.65930599369085</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>34.20752565564425</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>39.42181340341656</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>40.16064257028113</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>44.31314623338257</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>43.98826979472141</v>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>45.523520485584214</t>
         </is>
       </c>
     </row>
@@ -2595,23 +2915,38 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>32.71537622682661</v>
+        <v>3.000900270081024</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>33.86004514672686</v>
+        <v>5.90434953749262</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>31.61222339304531</v>
+        <v>9.77198697068404</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>30.58103975535168</v>
+        <v>15.600624024961</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>32.89473684210527</v>
-      </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>31.023784901758013</t>
+        <v>20.40816326530612</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>24.330900243309</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>28.59866539561488</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>30.3030303030303</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>28.40909090909091</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>29.49852507374631</v>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
+        <is>
+          <t>32.50270855904659</t>
         </is>
       </c>
     </row>
@@ -2620,23 +2955,38 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>24.01921537229784</v>
+        <v>3.181673560292713</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>24.11575562700965</v>
+        <v>5.866249511145874</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>24.25222312045271</v>
+        <v>10.04352192835621</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>24.81389578163772</v>
+        <v>14.55604075691412</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>22.53944402704733</v>
-      </c>
-      <c r="G5" s="2" t="inlineStr">
-        <is>
-          <t>23.006134969325153</t>
+        <v>18.65671641791045</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>21.56721782890008</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>22.72727272727273</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>22.86585365853659</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>23.45582486317436</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>22.38805970149254</v>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>24.63054187192118</t>
         </is>
       </c>
     </row>
@@ -2645,23 +2995,38 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>12.1654501216545</v>
+        <v>2.271436683702442</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>12.853470437018</v>
+        <v>3.181673560292714</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>13.05483028720627</v>
+        <v>4.282655246252677</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>12.95336787564767</v>
+        <v>5.347593582887701</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>12.63423878711308</v>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>13.054830287206267</t>
+        <v>6.749915626054674</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>7.939658594680429</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>9.017132551848512</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>10.44386422976501</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>10.92896174863388</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>11.19194180190263</v>
+      </c>
+      <c r="L6" s="2" t="inlineStr">
+        <is>
+          <t>12.338062924120914</t>
         </is>
       </c>
     </row>
@@ -2670,23 +3035,38 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>10.80497028633171</v>
+        <v>2.108592514496574</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>10.52631578947368</v>
+        <v>2.928686484111876</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>10.23017902813299</v>
+        <v>3.937783028155149</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>10.96491228070176</v>
+        <v>5.040322580645161</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>10.61007957559682</v>
-      </c>
-      <c r="G7" s="2" t="inlineStr">
-        <is>
-          <t>10.21450459652707</t>
+        <v>6.325110689437065</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>6.856359273225917</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>8.628127696289905</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>8.635578583765112</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>9.246417013407305</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>9.704027171276079</v>
+      </c>
+      <c r="L7" s="2" t="inlineStr">
+        <is>
+          <t>10.121457489878543</t>
         </is>
       </c>
     </row>
@@ -2695,23 +3075,38 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>9.062075215224286</v>
+        <v>2.023472278429785</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>9.1324200913242</v>
+        <v>2.833262501770789</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>9.354536950420954</v>
+        <v>3.676470588235294</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>9.474182851729038</v>
+        <v>4.479283314669653</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>8.861320336730174</v>
-      </c>
-      <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>8.896797153024911</t>
+        <v>5.675368898978434</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>6.724949562878279</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>7.196833393306945</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>7.827788649706457</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>8.186655751125665</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>8.517887563884157</v>
+      </c>
+      <c r="L8" s="2" t="inlineStr">
+        <is>
+          <t>8.710801393728223</t>
         </is>
       </c>
     </row>
@@ -2720,23 +3115,38 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>8.100445524503847</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>7.898894154818326</v>
+        <v>2.737850787132101</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>7.927070947284978</v>
+        <v>3.564427018356799</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>7.840062720501764</v>
+        <v>4.407227853680035</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>7.980845969672785</v>
-      </c>
-      <c r="G9" s="2" t="inlineStr">
-        <is>
-          <t>7.800312012480499</t>
+        <v>5.293806246691371</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>6.038647342995169</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>6.540222367560497</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>6.868131868131868</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>7.209805335255948</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>7.473841554559043</v>
+      </c>
+      <c r="L9" s="2" t="inlineStr">
+        <is>
+          <t>7.686395080707149</t>
         </is>
       </c>
     </row>
@@ -2745,23 +3155,38 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>7.11997152011392</v>
+        <v>2.022858298776171</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>7.0298769771529</v>
+        <v>2.750653280154037</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>6.814310051107325</v>
+        <v>3.499562554680665</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>6.983240223463687</v>
+        <v>4.291845493562231</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>7.02000702000702</v>
-      </c>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>6.934812760055478</t>
+        <v>5.035246727089628</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>5.497526113249038</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>6.099420555047271</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>6.215040397762586</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>6.576783952647156</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>6.591957811470007</v>
+      </c>
+      <c r="L10" s="2" t="inlineStr">
+        <is>
+          <t>7.00770847932726</t>
         </is>
       </c>
     </row>
@@ -2770,23 +3195,38 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>6.369426751592357</v>
+        <v>2.095996646405366</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>6.474587245063128</v>
+        <v>2.782028098483795</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>6.349206349206349</v>
+        <v>3.420557550880793</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>6.393861892583121</v>
+        <v>4.112687641373638</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>6.466214031684449</v>
-      </c>
-      <c r="G11" s="2" t="inlineStr">
-        <is>
-          <t>6.412311638345623</t>
+        <v>4.705882352941177</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>5.166623611469904</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>5.738880918220947</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>5.844535359438924</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>6.056935190793459</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>6.193868070610096</v>
+      </c>
+      <c r="L11" s="2" t="inlineStr">
+        <is>
+          <t>6.155740227762388</t>
         </is>
       </c>
     </row>
@@ -2795,23 +3235,38 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>5.868544600938967</v>
+        <v>2.197319270490002</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>5.790387955993052</v>
+        <v>2.849408747684856</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>5.824111822947001</v>
+        <v>3.527959075674722</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>5.788712011577424</v>
+        <v>4.083299305839118</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>5.873715124816447</v>
-      </c>
-      <c r="G12" s="2" t="inlineStr">
-        <is>
-          <t>5.941770647653001</t>
+        <v>4.596644449551827</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>4.915212582944212</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>5.302226935312832</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>5.364806866952789</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>5.534034311012729</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>5.748778384593274</v>
+      </c>
+      <c r="L12" s="2" t="inlineStr">
+        <is>
+          <t>5.603810591202017</t>
         </is>
       </c>
     </row>
@@ -2820,23 +3275,38 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>5.379236148466918</v>
+        <v>2.379819133745835</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>5.31632110579479</v>
+        <v>2.965159377316531</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>5.257623554153523</v>
+        <v>3.50938761186173</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>5.279831045406547</v>
+        <v>4.046944556859571</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>5.356186395286556</v>
-      </c>
-      <c r="G13" s="2" t="inlineStr">
-        <is>
-          <t>5.205622071837585</t>
+        <v>4.342162396873643</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>4.791566842357451</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>4.905567819475104</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>5.073566717402334</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>5.23149359142035</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>5.298013245033113</v>
+      </c>
+      <c r="L13" s="2" t="inlineStr">
+        <is>
+          <t>5.192107995846314</t>
         </is>
       </c>
     </row>
@@ -2845,23 +3315,38 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>5.078720162519045</v>
+        <v>2.594033722438392</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>4.915212582944212</v>
+        <v>3.160056881023858</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>4.950495049504951</v>
+        <v>3.583587170757929</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>4.929751047572098</v>
+        <v>3.900916715428126</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>4.9079754601227</v>
-      </c>
-      <c r="G14" s="2" t="inlineStr">
-        <is>
-          <t>4.88997555012225</t>
+        <v>4.278074866310161</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>4.475274110539271</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>4.63070155128502</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>4.694835680751174</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>4.747211013529552</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>4.981320049813201</v>
+      </c>
+      <c r="L14" s="2" t="inlineStr">
+        <is>
+          <t>4.918839153959666</t>
         </is>
       </c>
     </row>
@@ -2870,23 +3355,38 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>4.593477262287552</v>
+        <v>2.898550724637681</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>4.558924093913836</v>
+        <v>3.399048266485384</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>4.6072333563695</v>
+        <v>3.723701359150996</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>4.574565416285453</v>
+        <v>4.021717273275689</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>4.585052728106374</v>
-      </c>
-      <c r="G15" s="2" t="inlineStr">
-        <is>
-          <t>4.5850527281063735</t>
+        <v>4.247186239116585</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>4.315925766076823</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>4.464285714285714</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>4.462293618920125</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>4.495392222971455</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>4.578754578754578</v>
+      </c>
+      <c r="L15" s="2" t="inlineStr">
+        <is>
+          <t>4.483299708585519</t>
         </is>
       </c>
     </row>
@@ -2895,23 +3395,38 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>4.235493434985176</v>
+        <v>3.359086328518643</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>4.238186056367875</v>
+        <v>3.648303538854433</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>4.287245444801715</v>
+        <v>3.896356906292616</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>4.365858982754857</v>
+        <v>3.986446083316723</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>4.261666311527807</v>
-      </c>
-      <c r="G16" s="2" t="inlineStr">
-        <is>
-          <t>4.265301770100234</t>
+        <v>4.13992962119644</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>4.145077720207254</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>4.199916001679966</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>4.193751310547285</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>4.203446826397646</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>4.282655246252677</v>
+      </c>
+      <c r="L16" s="2" t="inlineStr">
+        <is>
+          <t>4.236390595212878</t>
         </is>
       </c>
     </row>
@@ -2920,23 +3435,38 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>3.957261574990107</v>
+        <v>3.983270264887473</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>3.96589331746976</v>
+        <v>4.020100502512562</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>3.947108742845865</v>
+        <v>4.035512510088782</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>4.030632809351068</v>
+        <v>4.046944556859571</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>4.002401440864519</v>
-      </c>
-      <c r="G17" s="2" t="inlineStr">
-        <is>
-          <t>4.021717273275689</t>
+        <v>4.012036108324975</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>4.013646397752358</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>3.959611958028113</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>3.927729772191673</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>3.940886699507389</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>4.029820672980052</v>
+      </c>
+      <c r="L17" s="2" t="inlineStr">
+        <is>
+          <t>4.0290088638195005</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
all Data upp to 6 qbits
</commit_message>
<xml_diff>
--- a/noise_Bitflip_1_to_6_qubits_pes.xlsx
+++ b/noise_Bitflip_1_to_6_qubits_pes.xlsx
@@ -15,6 +15,8 @@
     <sheet name="4qbit_oracle" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="5 qubits" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="5qbit_oracle" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="6 qubits" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="6qbit_oracle" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -588,6 +590,1266 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Number of Marked Items</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>0.0005 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>0.001 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>0.0015 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>0.002 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>0.0025 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>0.003 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>0.0035 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>0.004 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>0.0045000000000000005 noise level oracle calls</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>0.005 noise level oracle calls</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>246.9135802469136</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>377.3584905660377</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>382.1656050955414</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>431.6546762589928</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>397.3509933774834</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>402.6845637583893</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>368.0981595092025</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>394.7368421052631</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>365.8536585365854</v>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>372.67080745341616</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>65.57377049180327</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>125.3918495297806</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>139.3728222996516</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>134.2281879194631</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>114.9425287356322</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>108.695652173913</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>123.8390092879257</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>120.4819277108434</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>139.3728222996516</v>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>134.68013468013467</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>74.34944237918215</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>81.13590263691684</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>86.39308855291577</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>78.125</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>81.79959100204499</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>86.02150537634408</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>83.68200836820084</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>80.8080808080808</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>86.76789587852494</v>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>82.98755186721992</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>29.61500493583416</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>46.65629860031104</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>48.8599348534202</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>48.78048780487805</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>50.16722408026756</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>48.54368932038835</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>46.43962848297213</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>51.10732538330494</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>49.18032786885246</v>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>51.0204081632653</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>26.20087336244542</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>36.54080389768575</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>38.80983182406209</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>39.37007874015748</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>37.03703703703704</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>39.31847968545216</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>39.37007874015748</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>42.31311706629055</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>39.26701570680628</v>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>38.61003861003861</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>25.29510961214165</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>31.91489361702128</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>33.22259136212624</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>29.73240832507433</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>29.55665024630542</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>30.33367037411526</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>31.67898627243928</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>33.86004514672686</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>30.51881993896236</v>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>33.0760749724366</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>23.32814930015552</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>26.04166666666666</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>28.08988764044944</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>27.1985494106981</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>26.59574468085106</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>27.27272727272728</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>26.01908065915004</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>26.80965147453083</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>28.49002849002849</v>
+      </c>
+      <c r="K8" s="2" t="inlineStr">
+        <is>
+          <t>26.785714285714285</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>22.35469448584202</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>24.07704654895666</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>23.60346184107003</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>23.31002331002331</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>23.60346184107003</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>23.96166134185304</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>23.86634844868735</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>24.63054187192118</v>
+      </c>
+      <c r="K9" s="2" t="inlineStr">
+        <is>
+          <t>24.31118314424635</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>18.52995676343422</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>20.90592334494773</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>21.291696238467</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>21.06741573033708</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>20.89136490250696</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>21.23142250530785</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>21.26151665485472</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>21.05263157894737</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>21.45922746781116</v>
+      </c>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>21.58273381294964</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>8.120178643930167</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>11.91185229303157</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>12.07000603500302</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>12.7959053103007</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>12.86173633440514</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>12.72264631043257</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>12.49219237976265</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>13.14924391847469</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>12.84521515735389</v>
+      </c>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>12.861736334405144</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>7.044734061289186</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>10.50420168067227</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>11.26126126126126</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>11.50747986191024</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>11.60092807424594</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>11.883541295306</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>11.81334908446545</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>11.0803324099723</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>11.26760563380282</v>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>11.142061281337048</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>6.868131868131868</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>9.900990099009899</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>10.42752867570386</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>10.8695652173913</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>10.5708245243129</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>10.34661148473875</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>10.82251082251082</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>10.77005923532579</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>11.2739571589628</v>
+      </c>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>10.63264221158958</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>6.293266205160478</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>9.066183136899364</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>9.910802775024775</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>10.10611419909045</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>9.84251968503937</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>10.00500250125063</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>10.05025125628141</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>9.837678307919331</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>9.541984732824428</v>
+      </c>
+      <c r="K14" s="2" t="inlineStr">
+        <is>
+          <t>10.040160642570282</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>6.079027355623101</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>8.375209380234505</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>8.896797153024911</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>9.324009324009324</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>9.31098696461825</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>9.254974548819993</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>9.170105456212749</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>9.025270758122744</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>9.140767824497258</v>
+      </c>
+      <c r="K15" s="2" t="inlineStr">
+        <is>
+          <t>9.272137227630969</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>5.878894767783657</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>7.877116975187081</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>8.456659619450317</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>8.532423208191126</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>8.639308855291576</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>8.635578583765112</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>8.539709649871904</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>8.375209380234505</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>8.710801393728223</v>
+      </c>
+      <c r="K16" s="2" t="inlineStr">
+        <is>
+          <t>8.298755186721992</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>5.701254275940707</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>7.630675314765357</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>7.818608287724785</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>7.82472613458529</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>7.971303308090873</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>7.864726700747149</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>8.090614886731391</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>7.902015013828526</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>7.952286282306163</v>
+      </c>
+      <c r="K17" s="2" t="inlineStr">
+        <is>
+          <t>7.968127490039841</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>5.494505494505495</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>6.87757909215956</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>7.564296520423601</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>7.513148009015778</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>7.550018875047187</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>7.473841554559043</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>7.8125</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>7.423904974016333</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>7.328691828508611</v>
+      </c>
+      <c r="K18" s="2" t="inlineStr">
+        <is>
+          <t>7.532956685499058</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>5.254860746190226</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>6.87757909215956</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>7.037297677691766</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>7.104795737122558</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>7.092198581560283</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>7.140307033202427</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>7.256894049346879</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>6.927606511950121</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>7.012622720897616</v>
+      </c>
+      <c r="K19" s="2" t="inlineStr">
+        <is>
+          <t>7.114905727499111</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>5.186721991701245</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>6.480881399870382</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>6.512536633018561</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>6.568144499178982</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>6.668889629876626</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>6.626905235255136</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>6.633499170812604</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>6.856359273225917</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>6.688963210702341</v>
+      </c>
+      <c r="K20" s="2" t="inlineStr">
+        <is>
+          <t>6.894174422612892</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>4.993757802746567</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>6.169031462060457</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>6.267627702914447</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>6.397952655150352</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>6.238303181534622</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>6.600660066006601</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>6.406149903907751</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>6.538084341288003</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>6.341154090044388</v>
+      </c>
+      <c r="K21" s="2" t="inlineStr">
+        <is>
+          <t>6.367398917542184</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>4.82392667631452</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>5.717552887364208</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>5.984440454817475</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>5.908419497784343</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>5.917159763313609</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>6.086427267194157</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>6.125574272588056</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>6.075334143377885</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>6.103143118706134</v>
+      </c>
+      <c r="K22" s="2" t="inlineStr">
+        <is>
+          <t>6.127450980392157</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>4.747211013529552</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>5.651313930488839</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>6.007810153199159</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>5.871990604815032</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>5.740528128587831</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>5.722460658082976</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>5.859947260474656</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>5.715918833952558</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>5.830903790087463</v>
+      </c>
+      <c r="K23" s="2" t="inlineStr">
+        <is>
+          <t>5.788712011577424</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>4.655493482309125</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>5.405405405405405</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>5.445140212360468</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>5.592841163310962</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>5.430355688297584</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>5.537098560354374</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>5.608524957936063</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>5.509641873278237</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>5.465974309920743</v>
+      </c>
+      <c r="K24" s="2" t="inlineStr">
+        <is>
+          <t>5.610098176718092</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>4.574565416285453</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>5.336179295624333</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>5.232862375719519</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>5.357621216180016</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>5.217845030002609</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>5.238344683080147</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>5.382131324004305</v>
+      </c>
+      <c r="I25" s="2" t="n">
+        <v>5.309264666843642</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>5.357621216180016</v>
+      </c>
+      <c r="K25" s="2" t="inlineStr">
+        <is>
+          <t>5.403944879762227</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>4.564125969876769</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>5.011275369581559</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>5.186721991701245</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>5.177323323841574</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>5.103342689461598</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>5.26454330086865</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>5.104645227156713</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>5.020080321285141</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>5.073566717402334</v>
+      </c>
+      <c r="K26" s="2" t="inlineStr">
+        <is>
+          <t>5.064573309698658</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>4.318721658389117</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>4.821600771456123</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>4.847309743092584</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>4.950495049504951</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>5.044136191677175</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>4.829751267809708</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>4.932182490752158</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>5.008765339343852</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>4.863813229571984</v>
+      </c>
+      <c r="K27" s="2" t="inlineStr">
+        <is>
+          <t>5.020080321285141</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>4.393673110720562</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>4.723665564478035</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>4.795013186286262</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>4.814636494944632</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>4.687133817670494</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>4.706989879971758</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>4.612546125461255</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>4.706989879971758</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>4.731488052992666</v>
+      </c>
+      <c r="K28" s="2" t="inlineStr">
+        <is>
+          <t>4.700352526439483</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>4.194630872483222</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>4.493372275893058</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>4.571428571428571</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>4.44642063139173</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>4.575611988103409</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>4.693733865289838</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>4.571428571428571</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>4.702562896778744</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>4.649000464900047</v>
+      </c>
+      <c r="K29" s="2" t="inlineStr">
+        <is>
+          <t>4.555808656036446</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>4.191114836546522</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>4.382120946538125</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>4.404316229905307</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>4.360148245040332</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>4.477277815088426</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>4.392708104546453</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>4.482294935006723</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>4.415011037527594</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>4.466279589102278</v>
+      </c>
+      <c r="K30" s="2" t="inlineStr">
+        <is>
+          <t>4.45632798573975</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>4.12796697626419</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>4.225649693640397</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>4.337453914552158</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>4.174493842621582</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>4.264392324093817</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>4.21674045962471</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>4.275331338178709</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>4.301075268817204</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>4.223864836325237</v>
+      </c>
+      <c r="K31" s="2" t="inlineStr">
+        <is>
+          <t>4.25531914893617</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>4.068348250610252</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>4.111842105263158</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>4.170141784820684</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>4.125412541254126</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>4.083299305839118</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>4.157139887757223</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>4.149377593360996</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>4.213187276174426</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>4.186728072011723</v>
+      </c>
+      <c r="K32" s="2" t="inlineStr">
+        <is>
+          <t>4.184975936388366</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>3.947108742845865</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>4.030632809351068</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>3.958828186856691</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>4.018485031143259</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>3.98406374501992</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>3.954913980620922</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>4.004004004004004</v>
+      </c>
+      <c r="I33" s="2" t="n">
+        <v>4.005607850991388</v>
+      </c>
+      <c r="J33" s="2" t="n">
+        <v>4.00320256204964</v>
+      </c>
+      <c r="K33" s="2" t="inlineStr">
+        <is>
+          <t>4.068348250610252</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -3473,4 +4735,1264 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Number of Marked Items</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>0.0005 noise level</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>0.001 noise level</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>0.0015 noise level</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>0.002 noise level</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>0.0025 noise level</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>0.003 noise level</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>0.0035 noise level</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>0.004 noise level</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>0.0045000000000000005 noise level</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>0.005 noise level</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>1.6099999999999999</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>5.38</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>4.93</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>5.12</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>4.89</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>4.65</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>4.78</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>4.61</v>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>4.82</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>10.13</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>6.43</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>6.140000000000001</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>6.15</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>6.460000000000001</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>5.88</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>11.45</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>8.210000000000001</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>7.729999999999999</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>7.62</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>7.630000000000001</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>7.62</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>7.090000000000001</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>7.64</v>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>7.7700000000000005</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>11.86</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>9.029999999999999</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>10.09</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>10.15</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>9.890000000000001</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>9.470000000000001</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>8.859999999999999</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>9.83</v>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>12.86</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>11.52</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>10.68</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>11.03</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>11.28</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>11.53</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>11.19</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>10.53</v>
+      </c>
+      <c r="K8" s="2" t="inlineStr">
+        <is>
+          <t>11.200000000000001</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>13.42</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>12.46</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>12.71</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>12.87</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>12.71</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>12.52</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>12.57</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>12.18</v>
+      </c>
+      <c r="K9" s="2" t="inlineStr">
+        <is>
+          <t>12.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>16.19</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>14.35</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>14.09</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>14.24</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>14.36</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>14.13</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>14.11</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>14.25</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>13.98</v>
+      </c>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>13.900000000000002</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>24.63</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>16.79</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>16.57</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>15.63</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>15.55</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>15.72</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>16.01</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>15.21</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>15.57</v>
+      </c>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>15.55</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>28.39</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>19.04</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>17.76</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>17.38</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>17.24</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>16.83</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>16.93</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>18.05</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>17.75</v>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>17.95</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>29.12</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>20.2</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>19.18</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>18.4</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>18.92</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>19.33</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>18.48</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>18.57</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>17.74</v>
+      </c>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>18.81</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>31.78</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>22.06</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>20.18</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>19.79</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>20.32</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>19.9</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>20.33</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>20.96</v>
+      </c>
+      <c r="K14" s="2" t="inlineStr">
+        <is>
+          <t>19.919999999999998</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>32.9</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>23.88</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>22.48</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>21.45</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>21.48</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>21.61</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>21.81</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>22.16</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>21.88</v>
+      </c>
+      <c r="K15" s="2" t="inlineStr">
+        <is>
+          <t>21.57</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>34.02</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>25.39</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>23.65</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>23.44</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>23.15</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>23.16</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>23.42</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>23.88</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>22.96</v>
+      </c>
+      <c r="K16" s="2" t="inlineStr">
+        <is>
+          <t>24.099999999999998</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>35.08</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>26.21</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>25.58</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>25.56</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>25.09</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>25.43</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>24.72</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>25.31</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>25.15</v>
+      </c>
+      <c r="K17" s="2" t="inlineStr">
+        <is>
+          <t>25.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>36.4</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>29.08</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>26.44</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>26.62</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>26.49</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>26.76</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>25.6</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>26.94</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>27.29</v>
+      </c>
+      <c r="K18" s="2" t="inlineStr">
+        <is>
+          <t>26.55</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>38.06</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>29.08</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>28.42</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>28.15</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>28.01</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>27.56</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>28.87</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>28.52</v>
+      </c>
+      <c r="K19" s="2" t="inlineStr">
+        <is>
+          <t>28.110000000000003</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>38.56</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>30.86</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>30.71</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>30.45</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>29.99</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>30.18</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>30.15</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>29.17</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>29.9</v>
+      </c>
+      <c r="K20" s="2" t="inlineStr">
+        <is>
+          <t>29.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>40.05</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>32.42</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>31.91</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>31.26</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>32.06</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>30.3</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>31.22</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>30.59</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>31.54</v>
+      </c>
+      <c r="K21" s="2" t="inlineStr">
+        <is>
+          <t>31.41</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>41.46</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>34.98</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>33.42</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>33.85</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>32.86</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>32.65</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>32.92</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>32.77</v>
+      </c>
+      <c r="K22" s="2" t="inlineStr">
+        <is>
+          <t>32.64</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>42.13</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>35.39</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>33.29</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>34.06</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>34.84</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>34.95</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>34.13</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>34.99</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>34.3</v>
+      </c>
+      <c r="K23" s="2" t="inlineStr">
+        <is>
+          <t>34.55</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>42.96</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>36.73</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>35.76</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>36.83</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>35.66</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>36.3</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>36.59</v>
+      </c>
+      <c r="K24" s="2" t="inlineStr">
+        <is>
+          <t>35.65</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>43.72</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>37.48</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>38.22</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>37.33000000000001</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>38.33</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>38.18</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>37.16</v>
+      </c>
+      <c r="I25" s="2" t="n">
+        <v>37.67</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>37.33000000000001</v>
+      </c>
+      <c r="K25" s="2" t="inlineStr">
+        <is>
+          <t>37.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>43.82</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>39.91</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>38.56</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>38.63</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>39.19</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>37.99</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>39.18</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>39.84</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>39.42</v>
+      </c>
+      <c r="K26" s="2" t="inlineStr">
+        <is>
+          <t>39.489999999999995</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>46.31</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>41.48</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>41.26000000000001</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>40.40000000000001</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>39.65</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>41.41</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>40.55</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>39.93</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>41.12</v>
+      </c>
+      <c r="K27" s="2" t="inlineStr">
+        <is>
+          <t>39.839999999999996</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>45.52</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>42.34</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>41.71</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>41.54</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>42.67</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>42.49</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>43.36</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>42.49</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>42.27</v>
+      </c>
+      <c r="K28" s="2" t="inlineStr">
+        <is>
+          <t>42.55</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>47.68</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>44.51</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>43.75</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>44.98</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>43.71</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>42.61</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>43.75</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>42.53</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>43.02</v>
+      </c>
+      <c r="K29" s="2" t="inlineStr">
+        <is>
+          <t>43.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>47.72</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>45.64</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>45.87</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>44.67</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>45.53</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>44.62</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>45.3</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>44.78</v>
+      </c>
+      <c r="K30" s="2" t="inlineStr">
+        <is>
+          <t>44.879999999999995</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>48.45</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>47.33</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>46.11</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>47.91</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>46.9</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>47.43</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>46.78</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>47.35</v>
+      </c>
+      <c r="K31" s="2" t="inlineStr">
+        <is>
+          <t>47.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>49.16</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>48.64</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>47.96</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>48.48</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>48.98</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>48.11</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>48.2</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>47.47</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>47.77</v>
+      </c>
+      <c r="K32" s="2" t="inlineStr">
+        <is>
+          <t>47.79</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>50.67</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>49.62</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>50.52</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>49.77</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>50.2</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>50.57000000000001</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>49.95</v>
+      </c>
+      <c r="I33" s="2" t="n">
+        <v>49.93</v>
+      </c>
+      <c r="J33" s="2" t="n">
+        <v>49.96</v>
+      </c>
+      <c r="K33" s="2" t="inlineStr">
+        <is>
+          <t>49.16</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>